<commit_message>
Preparing charts for NPS.
</commit_message>
<xml_diff>
--- a/Output/DoD_Acq_Trends_Contracts.xlsx
+++ b/Output/DoD_Acq_Trends_Contracts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Users\Greg\Repositories\Vendor\Output\"/>
     </mc:Choice>
@@ -46,7 +46,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="408">
   <si>
     <t>Fiscal_Year</t>
   </si>
@@ -1285,14 +1285,44 @@
   <si>
     <t>OMB22_GDP20</t>
   </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>1991</t>
+  </si>
+  <si>
+    <t>1992</t>
+  </si>
+  <si>
+    <t>1993</t>
+  </si>
+  <si>
+    <t>1994</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="16">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-&quot;₩&quot;* #,##0.00_-;\-&quot;₩&quot;* #,##0.00_-;_-&quot;₩&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0\ ;\-#,##0\ ;"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
@@ -1596,7 +1626,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1017">
+  <cellXfs count="1172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -4465,6 +4495,471 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="10">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="11">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="12">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -29228,16 +29723,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="15" width="9.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="21" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="28" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="32" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="36" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="15" customWidth="true" hidden="true" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="18" max="21" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="22" max="28" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="29" max="32" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="33" max="36" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45">
@@ -32514,7 +33009,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AP31"/>
+  <dimension ref="A1:AT31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="14" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
@@ -32525,14 +33020,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
-    <col min="2" max="14" width="0" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="19" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="34" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="36" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="14" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
+    <col min="15" max="19" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="20" max="34" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="35" max="36" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="29" customFormat="1" ht="12.75">
@@ -33703,73 +34198,103 @@
       <c r="M14" s="185" t="s">
         <v>363</v>
       </c>
-      <c r="N14" s="191" t="s">
+      <c r="N14" s="1017" t="s">
         <v>363</v>
       </c>
-      <c r="O14" s="192" t="s">
+      <c r="O14" s="1018" t="s">
+        <v>398</v>
+      </c>
+      <c r="P14" s="1019" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q14" s="1020" t="s">
+        <v>400</v>
+      </c>
+      <c r="R14" s="1021" t="s">
+        <v>401</v>
+      </c>
+      <c r="S14" s="1022" t="s">
+        <v>402</v>
+      </c>
+      <c r="T14" s="1023" t="s">
+        <v>403</v>
+      </c>
+      <c r="U14" s="1024" t="s">
+        <v>404</v>
+      </c>
+      <c r="V14" s="1025" t="s">
+        <v>405</v>
+      </c>
+      <c r="W14" s="1026" t="s">
+        <v>406</v>
+      </c>
+      <c r="X14" s="1027" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y14" s="1028" t="s">
         <v>364</v>
       </c>
-      <c r="P14" s="193" t="s">
+      <c r="Z14" s="1029" t="s">
         <v>365</v>
       </c>
-      <c r="Q14" s="194" t="s">
+      <c r="AA14" s="1030" t="s">
         <v>366</v>
       </c>
-      <c r="R14" s="195" t="s">
+      <c r="AB14" s="1031" t="s">
         <v>367</v>
       </c>
-      <c r="S14" s="196" t="s">
+      <c r="AC14" s="1032" t="s">
         <v>368</v>
       </c>
-      <c r="T14" s="197" t="s">
+      <c r="AD14" s="1033" t="s">
         <v>369</v>
       </c>
-      <c r="U14" s="198" t="s">
+      <c r="AE14" s="1034" t="s">
         <v>370</v>
       </c>
-      <c r="V14" s="199" t="s">
+      <c r="AF14" s="1035" t="s">
         <v>371</v>
       </c>
-      <c r="W14" s="200" t="s">
+      <c r="AG14" s="1036" t="s">
         <v>372</v>
       </c>
-      <c r="X14" s="201" t="s">
+      <c r="AH14" s="1037" t="s">
         <v>373</v>
       </c>
-      <c r="Y14" s="202" t="s">
+      <c r="AI14" s="1038" t="s">
         <v>374</v>
       </c>
-      <c r="Z14" s="203" t="s">
+      <c r="AJ14" s="1039" t="s">
         <v>375</v>
       </c>
-      <c r="AA14" s="204" t="s">
+      <c r="AK14" t="s" s="1040">
         <v>376</v>
       </c>
-      <c r="AB14" s="205" t="s">
+      <c r="AL14" t="s" s="1041">
         <v>377</v>
       </c>
-      <c r="AC14" s="206" t="s">
+      <c r="AM14" t="s" s="1042">
         <v>378</v>
       </c>
-      <c r="AD14" s="207" t="s">
+      <c r="AN14" t="s" s="1043">
         <v>379</v>
       </c>
-      <c r="AE14" s="208" t="s">
+      <c r="AO14" t="s" s="1044">
         <v>380</v>
       </c>
-      <c r="AF14" s="209" t="s">
+      <c r="AP14" t="s" s="1045">
         <v>381</v>
       </c>
-      <c r="AG14" s="210" t="s">
+      <c r="AQ14" t="s" s="1046">
         <v>382</v>
       </c>
-      <c r="AH14" s="211" t="s">
+      <c r="AR14" t="s" s="1047">
         <v>383</v>
       </c>
-      <c r="AI14" s="212" t="s">
+      <c r="AS14" t="s" s="1048">
         <v>384</v>
       </c>
-      <c r="AJ14" s="213" t="s">
+      <c r="AT14" t="s" s="1049">
         <v>385</v>
       </c>
     </row>
@@ -33825,75 +34350,105 @@
         <f t="shared" si="0"/>
         <v>Products (All)</v>
       </c>
-      <c r="N15" s="214" t="str">
+      <c r="N15" s="1050" t="str">
         <f t="shared" si="0"/>
         <v>Products (All)</v>
       </c>
-      <c r="O15" s="218">
-        <v>59593906260.513397</v>
-      </c>
-      <c r="P15" s="222">
-        <v>65053356276.884102</v>
-      </c>
-      <c r="Q15" s="226">
-        <v>76867670916.124802</v>
-      </c>
-      <c r="R15" s="230">
-        <v>94880559227.124695</v>
-      </c>
-      <c r="S15" s="234">
-        <v>103835614735.6581</v>
-      </c>
-      <c r="T15" s="238">
-        <v>123380131431.71851</v>
-      </c>
-      <c r="U15" s="242">
-        <v>136259772874.5437</v>
-      </c>
-      <c r="V15" s="246">
-        <v>158474061509.50229</v>
-      </c>
-      <c r="W15" s="250">
-        <v>189951978660.7807</v>
-      </c>
-      <c r="X15" s="254">
-        <v>173587884989.14899</v>
-      </c>
-      <c r="Y15" s="258">
-        <v>161991727983.64359</v>
-      </c>
-      <c r="Z15" s="262">
-        <v>173047449802.0722</v>
-      </c>
-      <c r="AA15" s="266">
-        <v>171506005342.28839</v>
-      </c>
-      <c r="AB15" s="270">
-        <v>147621626020.737</v>
-      </c>
-      <c r="AC15" s="274">
-        <v>129279257849.1739</v>
-      </c>
-      <c r="AD15" s="277">
-        <v>129766723823.57271</v>
-      </c>
-      <c r="AE15" s="281">
-        <v>148615608115.37509</v>
-      </c>
-      <c r="AF15" s="285">
-        <v>163576431049.4324</v>
-      </c>
-      <c r="AG15" s="289">
-        <v>183110684115.8891</v>
-      </c>
-      <c r="AH15" s="293">
-        <v>193210819805.74329</v>
-      </c>
-      <c r="AI15" s="297">
-        <v>218072457331.68951</v>
-      </c>
-      <c r="AJ15" s="301">
-        <v>194222077002.18851</v>
+      <c r="O15" s="1054" t="n">
+        <v>6.8380721115E10</v>
+      </c>
+      <c r="P15" s="1058" t="n">
+        <v>7.3383395678E10</v>
+      </c>
+      <c r="Q15" s="1061" t="n">
+        <v>6.0090730088E10</v>
+      </c>
+      <c r="R15" s="1064" t="n">
+        <v>6.0299705534E10</v>
+      </c>
+      <c r="S15" s="1067" t="n">
+        <v>5.1512841085E10</v>
+      </c>
+      <c r="T15" s="1070" t="n">
+        <v>4.9691607958E10</v>
+      </c>
+      <c r="U15" s="1073" t="n">
+        <v>5.2193436723E10</v>
+      </c>
+      <c r="V15" s="1076" t="n">
+        <v>4.927878064E10</v>
+      </c>
+      <c r="W15" s="1079" t="n">
+        <v>4.8098195391E10</v>
+      </c>
+      <c r="X15" s="1082" t="n">
+        <v>5.1802770524E10</v>
+      </c>
+      <c r="Y15" s="1085" t="n">
+        <v>5.95939062605134E10</v>
+      </c>
+      <c r="Z15" s="1089" t="n">
+        <v>6.50533562768841E10</v>
+      </c>
+      <c r="AA15" s="1093" t="n">
+        <v>7.68676709161248E10</v>
+      </c>
+      <c r="AB15" s="1097" t="n">
+        <v>9.48805592271247E10</v>
+      </c>
+      <c r="AC15" s="1101" t="n">
+        <v>1.038356147356581E11</v>
+      </c>
+      <c r="AD15" s="1105" t="n">
+        <v>1.233801314317185E11</v>
+      </c>
+      <c r="AE15" s="1109" t="n">
+        <v>1.362597728745437E11</v>
+      </c>
+      <c r="AF15" s="1113" t="n">
+        <v>1.584740615095023E11</v>
+      </c>
+      <c r="AG15" s="1117" t="n">
+        <v>1.899519786607807E11</v>
+      </c>
+      <c r="AH15" s="1121" t="n">
+        <v>1.73587884989149E11</v>
+      </c>
+      <c r="AI15" s="1125" t="n">
+        <v>1.619917279836436E11</v>
+      </c>
+      <c r="AJ15" s="1129" t="n">
+        <v>1.730474498020722E11</v>
+      </c>
+      <c r="AK15" t="n" s="1133">
+        <v>1.715060053422884E11</v>
+      </c>
+      <c r="AL15" t="n" s="1137">
+        <v>1.47621626020737E11</v>
+      </c>
+      <c r="AM15" t="n" s="1141">
+        <v>1.292792578491739E11</v>
+      </c>
+      <c r="AN15" t="n" s="1144">
+        <v>1.2976672382357271E11</v>
+      </c>
+      <c r="AO15" t="n" s="1148">
+        <v>1.486156081153751E11</v>
+      </c>
+      <c r="AP15" t="n" s="1152">
+        <v>1.635764310494324E11</v>
+      </c>
+      <c r="AQ15" t="n" s="1156">
+        <v>1.831106841158891E11</v>
+      </c>
+      <c r="AR15" t="n" s="1160">
+        <v>1.932108198057433E11</v>
+      </c>
+      <c r="AS15" t="n" s="1164">
+        <v>2.180724573316895E11</v>
+      </c>
+      <c r="AT15" t="n" s="1168">
+        <v>1.942220770021885E11</v>
       </c>
     </row>
     <row r="16" spans="1:39" s="29" customFormat="1">
@@ -33948,75 +34503,105 @@
         <f t="shared" si="1"/>
         <v>R&amp;D</v>
       </c>
-      <c r="N16" s="215" t="str">
+      <c r="N16" s="1051" t="str">
         <f t="shared" si="1"/>
         <v>R&amp;D</v>
       </c>
-      <c r="O16" s="219">
-        <v>18975571688.195202</v>
-      </c>
-      <c r="P16" s="223">
-        <v>20659939450.0872</v>
-      </c>
-      <c r="Q16" s="227">
-        <v>24447959897.318298</v>
-      </c>
-      <c r="R16" s="231">
-        <v>28293381987.8419</v>
-      </c>
-      <c r="S16" s="235">
-        <v>29933848137.3657</v>
-      </c>
-      <c r="T16" s="239">
-        <v>34308479488.283798</v>
-      </c>
-      <c r="U16" s="243">
-        <v>37917799020.3451</v>
-      </c>
-      <c r="V16" s="247">
-        <v>40740659030.874496</v>
-      </c>
-      <c r="W16" s="251">
-        <v>39515918070.894402</v>
-      </c>
-      <c r="X16" s="255">
-        <v>41998376180.222298</v>
-      </c>
-      <c r="Y16" s="259">
-        <v>39753925416.627197</v>
-      </c>
-      <c r="Z16" s="263">
-        <v>37470739089.002899</v>
-      </c>
-      <c r="AA16" s="267">
-        <v>33395994906.279099</v>
-      </c>
-      <c r="AB16" s="271">
-        <v>26566746535.464001</v>
-      </c>
-      <c r="AC16" s="275">
-        <v>24194265869.928299</v>
-      </c>
-      <c r="AD16" s="278">
-        <v>22527325311.6689</v>
-      </c>
-      <c r="AE16" s="282">
-        <v>23414434474.478001</v>
-      </c>
-      <c r="AF16" s="286">
-        <v>24590720482.705399</v>
-      </c>
-      <c r="AG16" s="290">
-        <v>26150331530.954102</v>
-      </c>
-      <c r="AH16" s="294">
-        <v>29756218178.5443</v>
-      </c>
-      <c r="AI16" s="298">
-        <v>30219025303.333698</v>
-      </c>
-      <c r="AJ16" s="302">
-        <v>31432718613.424702</v>
+      <c r="O16" s="1055" t="n">
+        <v>2.0132124764E10</v>
+      </c>
+      <c r="P16" s="1059" t="n">
+        <v>1.9885713573E10</v>
+      </c>
+      <c r="Q16" s="1062" t="n">
+        <v>2.0567110455E10</v>
+      </c>
+      <c r="R16" s="1065" t="n">
+        <v>2.1162972669E10</v>
+      </c>
+      <c r="S16" s="1068" t="n">
+        <v>2.1362580777E10</v>
+      </c>
+      <c r="T16" s="1071" t="n">
+        <v>2.1473104298E10</v>
+      </c>
+      <c r="U16" s="1074" t="n">
+        <v>2.0037157373E10</v>
+      </c>
+      <c r="V16" s="1077" t="n">
+        <v>1.9437221946E10</v>
+      </c>
+      <c r="W16" s="1080" t="n">
+        <v>1.9780164014E10</v>
+      </c>
+      <c r="X16" s="1083" t="n">
+        <v>1.9040526682E10</v>
+      </c>
+      <c r="Y16" s="1086" t="n">
+        <v>1.89755716881952E10</v>
+      </c>
+      <c r="Z16" s="1090" t="n">
+        <v>2.06599394500872E10</v>
+      </c>
+      <c r="AA16" s="1094" t="n">
+        <v>2.44479598973183E10</v>
+      </c>
+      <c r="AB16" s="1098" t="n">
+        <v>2.82933819878419E10</v>
+      </c>
+      <c r="AC16" s="1102" t="n">
+        <v>2.99338481373657E10</v>
+      </c>
+      <c r="AD16" s="1106" t="n">
+        <v>3.43084794882838E10</v>
+      </c>
+      <c r="AE16" s="1110" t="n">
+        <v>3.79177990203451E10</v>
+      </c>
+      <c r="AF16" s="1114" t="n">
+        <v>4.07406590308745E10</v>
+      </c>
+      <c r="AG16" s="1118" t="n">
+        <v>3.95159180708944E10</v>
+      </c>
+      <c r="AH16" s="1122" t="n">
+        <v>4.19983761802223E10</v>
+      </c>
+      <c r="AI16" s="1126" t="n">
+        <v>3.97539254166272E10</v>
+      </c>
+      <c r="AJ16" s="1130" t="n">
+        <v>3.74707390890029E10</v>
+      </c>
+      <c r="AK16" t="n" s="1134">
+        <v>3.33959949062791E10</v>
+      </c>
+      <c r="AL16" t="n" s="1138">
+        <v>2.6566746535464E10</v>
+      </c>
+      <c r="AM16" t="n" s="1142">
+        <v>2.41942658699283E10</v>
+      </c>
+      <c r="AN16" t="n" s="1145">
+        <v>2.25273253116689E10</v>
+      </c>
+      <c r="AO16" t="n" s="1149">
+        <v>2.3414434474478E10</v>
+      </c>
+      <c r="AP16" t="n" s="1153">
+        <v>2.45907204827054E10</v>
+      </c>
+      <c r="AQ16" t="n" s="1157">
+        <v>2.61503315309541E10</v>
+      </c>
+      <c r="AR16" t="n" s="1161">
+        <v>2.97562181785443E10</v>
+      </c>
+      <c r="AS16" t="n" s="1165">
+        <v>3.02190253033337E10</v>
+      </c>
+      <c r="AT16" t="n" s="1169">
+        <v>3.14327186134247E10</v>
       </c>
     </row>
     <row r="17" spans="1:42" s="29" customFormat="1" ht="45">
@@ -34071,75 +34656,105 @@
         <f t="shared" si="2"/>
         <v>Services (Non-R&amp;D)</v>
       </c>
-      <c r="N17" s="216" t="str">
+      <c r="N17" s="1052" t="str">
         <f t="shared" si="2"/>
         <v>Services (Non-R&amp;D)</v>
       </c>
-      <c r="O17" s="220">
-        <v>53561991198.140198</v>
-      </c>
-      <c r="P17" s="224">
-        <v>58241719613.047096</v>
-      </c>
-      <c r="Q17" s="228">
-        <v>68359297809.015999</v>
-      </c>
-      <c r="R17" s="232">
-        <v>88281674997.9534</v>
-      </c>
-      <c r="S17" s="236">
-        <v>95849169698.045105</v>
-      </c>
-      <c r="T17" s="240">
-        <v>107812108344.1783</v>
-      </c>
-      <c r="U17" s="244">
-        <v>120796242708.62891</v>
-      </c>
-      <c r="V17" s="248">
-        <v>128733859261.14371</v>
-      </c>
-      <c r="W17" s="252">
-        <v>148186717515.03519</v>
-      </c>
-      <c r="X17" s="256">
-        <v>165494962883.5723</v>
-      </c>
-      <c r="Y17" s="260">
-        <v>160433378820.3725</v>
-      </c>
-      <c r="Z17" s="264">
-        <v>157656124489.7269</v>
-      </c>
-      <c r="AA17" s="268">
-        <v>152372994425.81689</v>
-      </c>
-      <c r="AB17" s="272">
-        <v>132073807550.00099</v>
-      </c>
-      <c r="AC17" s="276">
-        <v>129576837592.31059</v>
-      </c>
-      <c r="AD17" s="279">
-        <v>121638587936.974</v>
-      </c>
-      <c r="AE17" s="283">
-        <v>125996896028.1819</v>
-      </c>
-      <c r="AF17" s="287">
-        <v>132214929602.6804</v>
-      </c>
-      <c r="AG17" s="291">
-        <v>149371989508.138</v>
-      </c>
-      <c r="AH17" s="295">
-        <v>160584610111.2215</v>
-      </c>
-      <c r="AI17" s="299">
-        <v>173015852054.43301</v>
-      </c>
-      <c r="AJ17" s="303">
-        <v>160857964285.306</v>
+      <c r="O17" s="1056" t="n">
+        <v>3.1837283526E10</v>
+      </c>
+      <c r="P17" s="1060" t="n">
+        <v>4.2885084593E10</v>
+      </c>
+      <c r="Q17" s="1063" t="n">
+        <v>4.2748820007E10</v>
+      </c>
+      <c r="R17" s="1066" t="n">
+        <v>3.9910703939E10</v>
+      </c>
+      <c r="S17" s="1069" t="n">
+        <v>4.4286480863E10</v>
+      </c>
+      <c r="T17" s="1072" t="n">
+        <v>4.5427302612E10</v>
+      </c>
+      <c r="U17" s="1075" t="n">
+        <v>4.6218185002E10</v>
+      </c>
+      <c r="V17" s="1078" t="n">
+        <v>4.7266149293E10</v>
+      </c>
+      <c r="W17" s="1081" t="n">
+        <v>4.9087522762E10</v>
+      </c>
+      <c r="X17" s="1084" t="n">
+        <v>5.1341739282E10</v>
+      </c>
+      <c r="Y17" s="1087" t="n">
+        <v>5.35619911981402E10</v>
+      </c>
+      <c r="Z17" s="1091" t="n">
+        <v>5.82417196130471E10</v>
+      </c>
+      <c r="AA17" s="1095" t="n">
+        <v>6.8359297809016E10</v>
+      </c>
+      <c r="AB17" s="1099" t="n">
+        <v>8.82816749979534E10</v>
+      </c>
+      <c r="AC17" s="1103" t="n">
+        <v>9.58491696980451E10</v>
+      </c>
+      <c r="AD17" s="1107" t="n">
+        <v>1.078121083441783E11</v>
+      </c>
+      <c r="AE17" s="1111" t="n">
+        <v>1.207962427086289E11</v>
+      </c>
+      <c r="AF17" s="1115" t="n">
+        <v>1.287338592611437E11</v>
+      </c>
+      <c r="AG17" s="1119" t="n">
+        <v>1.481867175150352E11</v>
+      </c>
+      <c r="AH17" s="1123" t="n">
+        <v>1.654949628835723E11</v>
+      </c>
+      <c r="AI17" s="1127" t="n">
+        <v>1.604333788203725E11</v>
+      </c>
+      <c r="AJ17" s="1131" t="n">
+        <v>1.576561244897269E11</v>
+      </c>
+      <c r="AK17" t="n" s="1135">
+        <v>1.523729944258169E11</v>
+      </c>
+      <c r="AL17" t="n" s="1139">
+        <v>1.3207380755000099E11</v>
+      </c>
+      <c r="AM17" t="n" s="1143">
+        <v>1.295768375923106E11</v>
+      </c>
+      <c r="AN17" t="n" s="1146">
+        <v>1.21638587936974E11</v>
+      </c>
+      <c r="AO17" t="n" s="1150">
+        <v>1.259968960281819E11</v>
+      </c>
+      <c r="AP17" t="n" s="1154">
+        <v>1.322149296026804E11</v>
+      </c>
+      <c r="AQ17" t="n" s="1158">
+        <v>1.49371989508138E11</v>
+      </c>
+      <c r="AR17" t="n" s="1162">
+        <v>1.605846101112215E11</v>
+      </c>
+      <c r="AS17" t="n" s="1166">
+        <v>1.73015852054433E11</v>
+      </c>
+      <c r="AT17" t="n" s="1170">
+        <v>1.60857964285306E11</v>
       </c>
     </row>
     <row r="18" spans="1:42" s="29" customFormat="1" ht="30">
@@ -34182,72 +34797,84 @@
       <c r="M18" s="189" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="217" t="s">
+      <c r="N18" s="1053" t="s">
         <v>51</v>
       </c>
-      <c r="O18" s="221">
-        <v>29507158.538600001</v>
-      </c>
-      <c r="P18" s="225">
-        <v>9838575.9425000008</v>
-      </c>
-      <c r="Q18" s="229">
-        <v>84083862.295499995</v>
-      </c>
-      <c r="R18" s="233">
-        <v>75741000.173999995</v>
-      </c>
-      <c r="S18" s="237">
+      <c r="O18" s="1057" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P18" s="225"/>
+      <c r="Q18" s="229"/>
+      <c r="R18" s="233"/>
+      <c r="S18" s="237"/>
+      <c r="T18" s="241"/>
+      <c r="U18" s="245"/>
+      <c r="V18" s="249"/>
+      <c r="W18" s="253"/>
+      <c r="X18" s="257"/>
+      <c r="Y18" s="1088" t="n">
+        <v>2.95071585386E7</v>
+      </c>
+      <c r="Z18" s="1092" t="n">
+        <v>9838575.9425</v>
+      </c>
+      <c r="AA18" s="1096" t="n">
+        <v>8.40838622955E7</v>
+      </c>
+      <c r="AB18" s="1100" t="n">
+        <v>7.5741000174E7</v>
+      </c>
+      <c r="AC18" s="1104" t="n">
         <v>7078195.7826000005</v>
       </c>
-      <c r="T18" s="241">
-        <v>3802636.1222999999</v>
-      </c>
-      <c r="U18" s="245">
-        <v>109748294.80769999</v>
-      </c>
-      <c r="V18" s="249">
-        <v>18047585.049899999</v>
-      </c>
-      <c r="W18" s="253">
+      <c r="AD18" s="1108" t="n">
+        <v>3802636.1223</v>
+      </c>
+      <c r="AE18" s="1112" t="n">
+        <v>1.097482948077E8</v>
+      </c>
+      <c r="AF18" s="1116" t="n">
+        <v>1.80475850499E7</v>
+      </c>
+      <c r="AG18" s="1120" t="n">
         <v>368043.21920000005</v>
       </c>
-      <c r="X18" s="257">
-        <v>986168.13329999999</v>
-      </c>
-      <c r="Y18" s="261">
+      <c r="AH18" s="1124" t="n">
+        <v>986168.1333</v>
+      </c>
+      <c r="AI18" s="1128" t="n">
         <v>-253919.658</v>
       </c>
-      <c r="Z18" s="265">
-        <v>-140825.10130000001</v>
-      </c>
-      <c r="AA18" s="269">
-        <v>-6477.8001000000004</v>
-      </c>
-      <c r="AB18" s="273">
-        <v>-99723.120599999995</v>
-      </c>
-      <c r="AC18" s="190"/>
-      <c r="AD18" s="280">
-        <v>30000</v>
-      </c>
-      <c r="AE18" s="284">
-        <v>3581529.4308000002</v>
-      </c>
-      <c r="AF18" s="288">
-        <v>1345607</v>
-      </c>
-      <c r="AG18" s="292">
-        <v>-212795.36720000001</v>
-      </c>
-      <c r="AH18" s="296">
-        <v>465885</v>
-      </c>
-      <c r="AI18" s="300">
+      <c r="AJ18" s="1132" t="n">
+        <v>-140825.1013</v>
+      </c>
+      <c r="AK18" t="n" s="1136">
+        <v>-6477.8001</v>
+      </c>
+      <c r="AL18" t="n" s="1140">
+        <v>-99723.1206</v>
+      </c>
+      <c r="AM18"/>
+      <c r="AN18" t="n" s="1147">
+        <v>30000.0</v>
+      </c>
+      <c r="AO18" t="n" s="1151">
+        <v>3581529.4308</v>
+      </c>
+      <c r="AP18" t="n" s="1155">
+        <v>1345607.0</v>
+      </c>
+      <c r="AQ18" t="n" s="1159">
+        <v>-212795.3672</v>
+      </c>
+      <c r="AR18" t="n" s="1163">
+        <v>465885.0</v>
+      </c>
+      <c r="AS18" t="n" s="1167">
         <v>314555.625</v>
       </c>
-      <c r="AJ18" s="304">
-        <v>386316</v>
+      <c r="AT18" t="n" s="1171">
+        <v>386316.0</v>
       </c>
     </row>
     <row r="19" spans="1:42" s="29" customFormat="1" ht="12.75"/>
@@ -35066,13 +35693,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="14" width="0" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="35" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="38" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="14" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="17" max="35" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="37" max="38" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -36993,7 +37620,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
@@ -37004,8 +37631,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="22" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="22" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -38463,15 +39090,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1" collapsed="1"/>
-    <col min="2" max="13" width="9.140625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="28" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="29" max="35" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="9.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="52.0" collapsed="true"/>
+    <col min="2" max="13" customWidth="true" hidden="true" width="9.140625" collapsed="true"/>
+    <col min="14" max="28" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="29" max="35" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
@@ -40734,11 +41361,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="14" width="0" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="35" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="14" customWidth="true" hidden="true" width="0.0" collapsed="true"/>
+    <col min="15" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="32" max="35" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
@@ -44825,11 +45452,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="3.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -46688,9 +47315,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="2" max="16" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -48728,390 +49355,390 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="256" width="9" style="76" collapsed="1"/>
-    <col min="257" max="257" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="258" max="258" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="259" max="259" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="260" max="260" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="261" max="261" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="262" max="512" width="9" style="76" collapsed="1"/>
-    <col min="513" max="513" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="514" max="514" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="515" max="515" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="516" max="516" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="517" max="517" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="518" max="768" width="9" style="76" collapsed="1"/>
-    <col min="769" max="769" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="770" max="770" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="771" max="771" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="772" max="772" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="773" max="773" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="774" max="1024" width="9" style="76" collapsed="1"/>
-    <col min="1025" max="1025" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1026" max="1026" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1027" max="1027" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1028" max="1028" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1029" max="1029" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1030" max="1280" width="9" style="76" collapsed="1"/>
-    <col min="1281" max="1281" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1282" max="1282" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1283" max="1283" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1284" max="1284" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1285" max="1285" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1286" max="1536" width="9" style="76" collapsed="1"/>
-    <col min="1537" max="1537" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1538" max="1538" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1539" max="1539" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1540" max="1540" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1541" max="1541" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1542" max="1792" width="9" style="76" collapsed="1"/>
-    <col min="1793" max="1793" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1794" max="1794" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1795" max="1795" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1796" max="1796" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1797" max="1797" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="1798" max="2048" width="9" style="76" collapsed="1"/>
-    <col min="2049" max="2049" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2050" max="2050" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2051" max="2051" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2052" max="2052" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2053" max="2053" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2054" max="2304" width="9" style="76" collapsed="1"/>
-    <col min="2305" max="2305" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2306" max="2306" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2307" max="2307" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2308" max="2308" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2309" max="2309" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2310" max="2560" width="9" style="76" collapsed="1"/>
-    <col min="2561" max="2561" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2562" max="2562" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2563" max="2563" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2564" max="2564" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2565" max="2565" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2566" max="2816" width="9" style="76" collapsed="1"/>
-    <col min="2817" max="2817" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2818" max="2818" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2819" max="2819" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2820" max="2820" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2821" max="2821" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2822" max="3072" width="9" style="76" collapsed="1"/>
-    <col min="3073" max="3073" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3074" max="3074" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3075" max="3075" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3076" max="3076" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3077" max="3077" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3078" max="3328" width="9" style="76" collapsed="1"/>
-    <col min="3329" max="3329" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3330" max="3330" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3331" max="3331" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3332" max="3332" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3333" max="3333" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3334" max="3584" width="9" style="76" collapsed="1"/>
-    <col min="3585" max="3585" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3586" max="3586" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3587" max="3587" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3588" max="3588" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3589" max="3589" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3590" max="3840" width="9" style="76" collapsed="1"/>
-    <col min="3841" max="3841" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3842" max="3842" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3843" max="3843" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3844" max="3844" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3845" max="3845" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3846" max="4096" width="9" style="76" collapsed="1"/>
-    <col min="4097" max="4097" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4098" max="4098" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4099" max="4099" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4100" max="4100" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4101" max="4101" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4102" max="4352" width="9" style="76" collapsed="1"/>
-    <col min="4353" max="4353" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4354" max="4354" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4355" max="4355" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4356" max="4356" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4357" max="4357" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4358" max="4608" width="9" style="76" collapsed="1"/>
-    <col min="4609" max="4609" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4610" max="4610" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4611" max="4611" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4612" max="4612" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4613" max="4613" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4614" max="4864" width="9" style="76" collapsed="1"/>
-    <col min="4865" max="4865" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4866" max="4866" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4867" max="4867" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4868" max="4868" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4869" max="4869" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4870" max="5120" width="9" style="76" collapsed="1"/>
-    <col min="5121" max="5121" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5122" max="5122" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5123" max="5123" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5124" max="5124" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5125" max="5125" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5126" max="5376" width="9" style="76" collapsed="1"/>
-    <col min="5377" max="5377" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5378" max="5378" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5379" max="5379" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5380" max="5380" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5381" max="5381" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5382" max="5632" width="9" style="76" collapsed="1"/>
-    <col min="5633" max="5633" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5634" max="5634" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5635" max="5635" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5636" max="5636" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5637" max="5637" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5638" max="5888" width="9" style="76" collapsed="1"/>
-    <col min="5889" max="5889" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5890" max="5890" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5891" max="5891" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5892" max="5892" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5893" max="5893" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5894" max="6144" width="9" style="76" collapsed="1"/>
-    <col min="6145" max="6145" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6146" max="6146" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6147" max="6147" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6148" max="6148" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6149" max="6149" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6150" max="6400" width="9" style="76" collapsed="1"/>
-    <col min="6401" max="6401" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6402" max="6402" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6403" max="6403" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6404" max="6404" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6405" max="6405" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6406" max="6656" width="9" style="76" collapsed="1"/>
-    <col min="6657" max="6657" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6658" max="6658" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6659" max="6659" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6660" max="6660" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6661" max="6661" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6662" max="6912" width="9" style="76" collapsed="1"/>
-    <col min="6913" max="6913" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6914" max="6914" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6915" max="6915" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6916" max="6916" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6917" max="6917" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6918" max="7168" width="9" style="76" collapsed="1"/>
-    <col min="7169" max="7169" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7170" max="7170" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7171" max="7171" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7172" max="7172" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7173" max="7173" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7174" max="7424" width="9" style="76" collapsed="1"/>
-    <col min="7425" max="7425" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7426" max="7426" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7427" max="7427" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7428" max="7428" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7429" max="7429" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7430" max="7680" width="9" style="76" collapsed="1"/>
-    <col min="7681" max="7681" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7682" max="7682" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7683" max="7683" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7684" max="7684" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7685" max="7685" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7686" max="7936" width="9" style="76" collapsed="1"/>
-    <col min="7937" max="7937" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7938" max="7938" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7939" max="7939" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7940" max="7940" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7941" max="7941" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7942" max="8192" width="9" style="76" collapsed="1"/>
-    <col min="8193" max="8193" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8194" max="8194" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8195" max="8195" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8196" max="8196" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8197" max="8197" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8198" max="8448" width="9" style="76" collapsed="1"/>
-    <col min="8449" max="8449" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8450" max="8450" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8451" max="8451" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8452" max="8452" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8453" max="8453" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8454" max="8704" width="9" style="76" collapsed="1"/>
-    <col min="8705" max="8705" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8706" max="8706" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8707" max="8707" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8708" max="8708" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8709" max="8709" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8710" max="8960" width="9" style="76" collapsed="1"/>
-    <col min="8961" max="8961" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8962" max="8962" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8963" max="8963" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8964" max="8964" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8965" max="8965" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8966" max="9216" width="9" style="76" collapsed="1"/>
-    <col min="9217" max="9217" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9218" max="9218" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9219" max="9219" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9220" max="9220" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9221" max="9221" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9222" max="9472" width="9" style="76" collapsed="1"/>
-    <col min="9473" max="9473" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9474" max="9474" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9475" max="9475" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9476" max="9476" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9477" max="9477" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9478" max="9728" width="9" style="76" collapsed="1"/>
-    <col min="9729" max="9729" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9730" max="9730" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9731" max="9731" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9732" max="9732" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9733" max="9733" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9734" max="9984" width="9" style="76" collapsed="1"/>
-    <col min="9985" max="9985" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9986" max="9986" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9987" max="9987" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9988" max="9988" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9989" max="9989" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9990" max="10240" width="9" style="76" collapsed="1"/>
-    <col min="10241" max="10241" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10242" max="10242" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10243" max="10243" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10244" max="10244" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10245" max="10245" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10246" max="10496" width="9" style="76" collapsed="1"/>
-    <col min="10497" max="10497" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10498" max="10498" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10499" max="10499" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10500" max="10500" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10501" max="10501" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10502" max="10752" width="9" style="76" collapsed="1"/>
-    <col min="10753" max="10753" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10754" max="10754" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10755" max="10755" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10756" max="10756" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10757" max="10757" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10758" max="11008" width="9" style="76" collapsed="1"/>
-    <col min="11009" max="11009" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11010" max="11010" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11011" max="11011" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11012" max="11012" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11013" max="11013" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11014" max="11264" width="9" style="76" collapsed="1"/>
-    <col min="11265" max="11265" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11266" max="11266" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11267" max="11267" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11268" max="11268" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11269" max="11269" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11270" max="11520" width="9" style="76" collapsed="1"/>
-    <col min="11521" max="11521" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11522" max="11522" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11523" max="11523" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11524" max="11524" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11525" max="11525" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11526" max="11776" width="9" style="76" collapsed="1"/>
-    <col min="11777" max="11777" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11778" max="11778" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11779" max="11779" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11780" max="11780" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11781" max="11781" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11782" max="12032" width="9" style="76" collapsed="1"/>
-    <col min="12033" max="12033" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12034" max="12034" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12035" max="12035" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12036" max="12036" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12037" max="12037" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12038" max="12288" width="9" style="76" collapsed="1"/>
-    <col min="12289" max="12289" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12290" max="12290" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12291" max="12291" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12292" max="12292" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12293" max="12293" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12294" max="12544" width="9" style="76" collapsed="1"/>
-    <col min="12545" max="12545" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12546" max="12546" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12547" max="12547" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12548" max="12548" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12549" max="12549" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12550" max="12800" width="9" style="76" collapsed="1"/>
-    <col min="12801" max="12801" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12802" max="12802" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12803" max="12803" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12804" max="12804" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12805" max="12805" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12806" max="13056" width="9" style="76" collapsed="1"/>
-    <col min="13057" max="13057" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13058" max="13058" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13059" max="13059" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13060" max="13060" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13061" max="13061" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13062" max="13312" width="9" style="76" collapsed="1"/>
-    <col min="13313" max="13313" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13314" max="13314" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13315" max="13315" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13316" max="13316" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13317" max="13317" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13318" max="13568" width="9" style="76" collapsed="1"/>
-    <col min="13569" max="13569" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13570" max="13570" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13571" max="13571" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13572" max="13572" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13573" max="13573" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13574" max="13824" width="9" style="76" collapsed="1"/>
-    <col min="13825" max="13825" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13826" max="13826" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13827" max="13827" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13828" max="13828" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13829" max="13829" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13830" max="14080" width="9" style="76" collapsed="1"/>
-    <col min="14081" max="14081" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14082" max="14082" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14083" max="14083" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14084" max="14084" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14085" max="14085" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14086" max="14336" width="9" style="76" collapsed="1"/>
-    <col min="14337" max="14337" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14338" max="14338" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14339" max="14339" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14340" max="14340" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14341" max="14341" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14342" max="14592" width="9" style="76" collapsed="1"/>
-    <col min="14593" max="14593" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14594" max="14594" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14595" max="14595" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14596" max="14596" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14597" max="14597" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14598" max="14848" width="9" style="76" collapsed="1"/>
-    <col min="14849" max="14849" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14850" max="14850" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14851" max="14851" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14852" max="14852" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14853" max="14853" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14854" max="15104" width="9" style="76" collapsed="1"/>
-    <col min="15105" max="15105" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15106" max="15106" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15107" max="15107" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15108" max="15108" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15109" max="15109" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15110" max="15360" width="9" style="76" collapsed="1"/>
-    <col min="15361" max="15361" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15362" max="15362" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15363" max="15363" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15364" max="15364" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15365" max="15365" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15366" max="15616" width="9" style="76" collapsed="1"/>
-    <col min="15617" max="15617" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15618" max="15618" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15619" max="15619" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15620" max="15620" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15621" max="15621" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15622" max="15872" width="9" style="76" collapsed="1"/>
-    <col min="15873" max="15873" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15874" max="15874" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15875" max="15875" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15876" max="15876" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15877" max="15877" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15878" max="16128" width="9" style="76" collapsed="1"/>
-    <col min="16129" max="16129" width="66.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16130" max="16130" width="22.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16131" max="16131" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16132" max="16132" width="18.85546875" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16133" max="16133" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16134" max="16384" width="9" style="76" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="6" max="256" style="76" width="9.0" collapsed="true"/>
+    <col min="257" max="257" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="258" max="258" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="259" max="259" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="260" max="260" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="261" max="261" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="262" max="512" style="76" width="9.0" collapsed="true"/>
+    <col min="513" max="513" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="514" max="514" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="515" max="515" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="516" max="516" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="517" max="517" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="518" max="768" style="76" width="9.0" collapsed="true"/>
+    <col min="769" max="769" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="770" max="770" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="771" max="771" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="772" max="772" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="773" max="773" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="774" max="1024" style="76" width="9.0" collapsed="true"/>
+    <col min="1025" max="1025" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="1026" max="1026" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="1027" max="1027" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="1028" max="1028" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="1029" max="1029" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="1030" max="1280" style="76" width="9.0" collapsed="true"/>
+    <col min="1281" max="1281" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="1282" max="1282" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="1283" max="1283" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="1284" max="1284" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="1285" max="1285" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="1286" max="1536" style="76" width="9.0" collapsed="true"/>
+    <col min="1537" max="1537" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="1538" max="1538" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="1539" max="1539" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="1540" max="1540" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="1541" max="1541" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="1542" max="1792" style="76" width="9.0" collapsed="true"/>
+    <col min="1793" max="1793" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="1794" max="1794" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="1795" max="1795" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="1796" max="1796" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="1797" max="1797" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="1798" max="2048" style="76" width="9.0" collapsed="true"/>
+    <col min="2049" max="2049" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="2050" max="2050" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="2051" max="2051" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="2052" max="2052" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="2053" max="2053" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="2054" max="2304" style="76" width="9.0" collapsed="true"/>
+    <col min="2305" max="2305" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="2306" max="2306" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="2307" max="2307" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="2308" max="2308" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="2309" max="2309" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="2310" max="2560" style="76" width="9.0" collapsed="true"/>
+    <col min="2561" max="2561" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="2562" max="2562" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="2563" max="2563" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="2564" max="2564" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="2565" max="2565" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="2566" max="2816" style="76" width="9.0" collapsed="true"/>
+    <col min="2817" max="2817" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="2818" max="2818" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="2819" max="2819" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="2820" max="2820" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="2821" max="2821" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="2822" max="3072" style="76" width="9.0" collapsed="true"/>
+    <col min="3073" max="3073" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="3074" max="3074" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="3075" max="3075" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="3076" max="3076" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="3077" max="3077" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="3078" max="3328" style="76" width="9.0" collapsed="true"/>
+    <col min="3329" max="3329" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="3330" max="3330" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="3331" max="3331" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="3332" max="3332" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="3333" max="3333" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="3334" max="3584" style="76" width="9.0" collapsed="true"/>
+    <col min="3585" max="3585" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="3586" max="3586" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="3587" max="3587" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="3588" max="3588" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="3589" max="3589" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="3590" max="3840" style="76" width="9.0" collapsed="true"/>
+    <col min="3841" max="3841" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="3842" max="3842" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="3843" max="3843" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="3844" max="3844" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="3845" max="3845" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="3846" max="4096" style="76" width="9.0" collapsed="true"/>
+    <col min="4097" max="4097" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="4098" max="4098" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="4099" max="4099" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="4100" max="4100" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="4101" max="4101" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="4102" max="4352" style="76" width="9.0" collapsed="true"/>
+    <col min="4353" max="4353" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="4354" max="4354" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="4355" max="4355" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="4356" max="4356" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="4357" max="4357" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="4358" max="4608" style="76" width="9.0" collapsed="true"/>
+    <col min="4609" max="4609" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="4610" max="4610" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="4611" max="4611" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="4612" max="4612" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="4613" max="4613" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="4614" max="4864" style="76" width="9.0" collapsed="true"/>
+    <col min="4865" max="4865" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="4866" max="4866" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="4867" max="4867" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="4868" max="4868" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="4869" max="4869" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="4870" max="5120" style="76" width="9.0" collapsed="true"/>
+    <col min="5121" max="5121" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="5122" max="5122" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="5123" max="5123" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="5124" max="5124" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="5125" max="5125" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="5126" max="5376" style="76" width="9.0" collapsed="true"/>
+    <col min="5377" max="5377" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="5378" max="5378" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="5379" max="5379" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="5380" max="5380" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="5381" max="5381" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="5382" max="5632" style="76" width="9.0" collapsed="true"/>
+    <col min="5633" max="5633" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="5634" max="5634" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="5635" max="5635" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="5636" max="5636" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="5637" max="5637" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="5638" max="5888" style="76" width="9.0" collapsed="true"/>
+    <col min="5889" max="5889" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="5890" max="5890" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="5891" max="5891" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="5892" max="5892" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="5893" max="5893" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="5894" max="6144" style="76" width="9.0" collapsed="true"/>
+    <col min="6145" max="6145" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="6146" max="6146" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="6147" max="6147" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="6148" max="6148" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="6149" max="6149" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="6150" max="6400" style="76" width="9.0" collapsed="true"/>
+    <col min="6401" max="6401" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="6402" max="6402" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="6403" max="6403" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="6404" max="6404" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="6405" max="6405" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="6406" max="6656" style="76" width="9.0" collapsed="true"/>
+    <col min="6657" max="6657" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="6658" max="6658" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="6659" max="6659" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="6660" max="6660" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="6661" max="6661" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="6662" max="6912" style="76" width="9.0" collapsed="true"/>
+    <col min="6913" max="6913" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="6914" max="6914" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="6915" max="6915" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="6916" max="6916" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="6917" max="6917" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="6918" max="7168" style="76" width="9.0" collapsed="true"/>
+    <col min="7169" max="7169" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="7170" max="7170" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="7171" max="7171" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="7172" max="7172" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="7173" max="7173" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="7174" max="7424" style="76" width="9.0" collapsed="true"/>
+    <col min="7425" max="7425" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="7426" max="7426" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="7427" max="7427" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="7428" max="7428" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="7429" max="7429" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="7430" max="7680" style="76" width="9.0" collapsed="true"/>
+    <col min="7681" max="7681" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="7682" max="7682" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="7683" max="7683" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="7684" max="7684" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="7685" max="7685" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="7686" max="7936" style="76" width="9.0" collapsed="true"/>
+    <col min="7937" max="7937" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="7938" max="7938" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="7939" max="7939" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="7940" max="7940" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="7941" max="7941" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="7942" max="8192" style="76" width="9.0" collapsed="true"/>
+    <col min="8193" max="8193" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="8194" max="8194" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="8195" max="8195" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="8196" max="8196" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="8197" max="8197" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="8198" max="8448" style="76" width="9.0" collapsed="true"/>
+    <col min="8449" max="8449" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="8450" max="8450" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="8451" max="8451" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="8452" max="8452" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="8453" max="8453" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="8454" max="8704" style="76" width="9.0" collapsed="true"/>
+    <col min="8705" max="8705" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="8706" max="8706" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="8707" max="8707" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="8708" max="8708" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="8709" max="8709" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="8710" max="8960" style="76" width="9.0" collapsed="true"/>
+    <col min="8961" max="8961" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="8962" max="8962" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="8963" max="8963" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="8964" max="8964" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="8965" max="8965" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="8966" max="9216" style="76" width="9.0" collapsed="true"/>
+    <col min="9217" max="9217" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="9218" max="9218" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="9219" max="9219" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="9220" max="9220" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="9221" max="9221" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="9222" max="9472" style="76" width="9.0" collapsed="true"/>
+    <col min="9473" max="9473" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="9474" max="9474" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="9475" max="9475" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="9476" max="9476" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="9477" max="9477" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="9478" max="9728" style="76" width="9.0" collapsed="true"/>
+    <col min="9729" max="9729" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="9730" max="9730" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="9731" max="9731" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="9732" max="9732" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="9733" max="9733" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="9734" max="9984" style="76" width="9.0" collapsed="true"/>
+    <col min="9985" max="9985" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="9986" max="9986" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="9987" max="9987" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="9988" max="9988" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="9989" max="9989" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="9990" max="10240" style="76" width="9.0" collapsed="true"/>
+    <col min="10241" max="10241" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="10242" max="10242" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="10243" max="10243" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="10244" max="10244" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="10245" max="10245" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="10246" max="10496" style="76" width="9.0" collapsed="true"/>
+    <col min="10497" max="10497" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="10498" max="10498" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="10499" max="10499" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="10500" max="10500" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="10501" max="10501" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="10502" max="10752" style="76" width="9.0" collapsed="true"/>
+    <col min="10753" max="10753" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="10754" max="10754" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="10755" max="10755" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="10756" max="10756" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="10757" max="10757" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="10758" max="11008" style="76" width="9.0" collapsed="true"/>
+    <col min="11009" max="11009" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="11010" max="11010" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="11011" max="11011" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="11012" max="11012" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="11013" max="11013" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="11014" max="11264" style="76" width="9.0" collapsed="true"/>
+    <col min="11265" max="11265" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="11266" max="11266" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="11267" max="11267" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="11268" max="11268" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="11269" max="11269" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="11270" max="11520" style="76" width="9.0" collapsed="true"/>
+    <col min="11521" max="11521" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="11522" max="11522" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="11523" max="11523" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="11524" max="11524" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="11525" max="11525" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="11526" max="11776" style="76" width="9.0" collapsed="true"/>
+    <col min="11777" max="11777" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="11778" max="11778" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="11779" max="11779" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="11780" max="11780" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="11781" max="11781" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="11782" max="12032" style="76" width="9.0" collapsed="true"/>
+    <col min="12033" max="12033" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="12034" max="12034" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="12035" max="12035" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="12036" max="12036" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="12037" max="12037" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="12038" max="12288" style="76" width="9.0" collapsed="true"/>
+    <col min="12289" max="12289" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="12290" max="12290" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="12291" max="12291" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="12292" max="12292" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="12293" max="12293" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="12294" max="12544" style="76" width="9.0" collapsed="true"/>
+    <col min="12545" max="12545" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="12546" max="12546" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="12547" max="12547" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="12548" max="12548" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="12549" max="12549" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="12550" max="12800" style="76" width="9.0" collapsed="true"/>
+    <col min="12801" max="12801" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="12802" max="12802" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="12803" max="12803" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="12804" max="12804" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="12805" max="12805" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="12806" max="13056" style="76" width="9.0" collapsed="true"/>
+    <col min="13057" max="13057" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="13058" max="13058" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="13059" max="13059" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="13060" max="13060" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="13061" max="13061" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="13062" max="13312" style="76" width="9.0" collapsed="true"/>
+    <col min="13313" max="13313" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="13314" max="13314" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="13315" max="13315" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="13316" max="13316" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="13317" max="13317" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="13318" max="13568" style="76" width="9.0" collapsed="true"/>
+    <col min="13569" max="13569" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="13570" max="13570" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="13571" max="13571" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="13572" max="13572" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="13573" max="13573" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="13574" max="13824" style="76" width="9.0" collapsed="true"/>
+    <col min="13825" max="13825" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="13826" max="13826" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="13827" max="13827" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="13828" max="13828" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="13829" max="13829" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="13830" max="14080" style="76" width="9.0" collapsed="true"/>
+    <col min="14081" max="14081" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="14082" max="14082" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="14083" max="14083" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="14084" max="14084" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="14085" max="14085" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="14086" max="14336" style="76" width="9.0" collapsed="true"/>
+    <col min="14337" max="14337" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="14338" max="14338" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="14339" max="14339" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="14340" max="14340" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="14341" max="14341" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="14342" max="14592" style="76" width="9.0" collapsed="true"/>
+    <col min="14593" max="14593" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="14594" max="14594" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="14595" max="14595" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="14596" max="14596" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="14597" max="14597" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="14598" max="14848" style="76" width="9.0" collapsed="true"/>
+    <col min="14849" max="14849" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="14850" max="14850" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="14851" max="14851" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="14852" max="14852" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="14853" max="14853" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="14854" max="15104" style="76" width="9.0" collapsed="true"/>
+    <col min="15105" max="15105" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="15106" max="15106" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="15107" max="15107" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="15108" max="15108" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="15109" max="15109" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="15110" max="15360" style="76" width="9.0" collapsed="true"/>
+    <col min="15361" max="15361" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="15362" max="15362" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="15363" max="15363" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="15364" max="15364" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="15365" max="15365" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="15366" max="15616" style="76" width="9.0" collapsed="true"/>
+    <col min="15617" max="15617" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="15618" max="15618" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="15619" max="15619" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="15620" max="15620" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="15621" max="15621" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="15622" max="15872" style="76" width="9.0" collapsed="true"/>
+    <col min="15873" max="15873" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="15874" max="15874" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="15875" max="15875" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="15876" max="15876" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="15877" max="15877" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="15878" max="16128" style="76" width="9.0" collapsed="true"/>
+    <col min="16129" max="16129" bestFit="true" customWidth="true" style="76" width="66.5703125" collapsed="true"/>
+    <col min="16130" max="16130" bestFit="true" customWidth="true" style="76" width="22.42578125" collapsed="true"/>
+    <col min="16131" max="16131" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="16132" max="16132" bestFit="true" customWidth="true" style="76" width="18.85546875" collapsed="true"/>
+    <col min="16133" max="16133" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="16134" max="16384" style="76" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -50857,14 +51484,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="59.140625" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.42578125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.28515625" style="89" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" style="81" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" style="81" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9" style="76" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" style="76" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="76" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="76" width="59.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="76" width="21.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="89" width="20.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="81" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="81" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" style="76" width="9.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="76" width="18.5703125" collapsed="true"/>
+    <col min="8" max="16384" style="76" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -52634,15 +53261,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="8" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="15" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="19" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="5" max="8" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="15" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="16" max="19" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="20" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -55285,13 +55912,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.7109375" style="90" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="21.42578125" style="90" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" style="90" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.28515625" style="90" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" style="90" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" style="90" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9" style="90" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="90" width="73.7109375" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="90" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="90" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="90" width="18.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="90" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="90" width="20.7109375" collapsed="true"/>
+    <col min="8" max="16384" style="90" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -59012,8 +59639,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="22" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="22" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:26">
@@ -60339,7 +60966,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="23" max="24" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -60934,12 +61561,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.42578125" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -62702,12 +63329,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.42578125" style="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="23" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="21" width="28.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="5" max="23" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -64161,28 +64788,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:22">
@@ -65840,15 +66467,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="23" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="23" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -69247,15 +69874,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="23" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="23" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">

</xml_diff>